<commit_message>
subida Miercoles 22 marzo
</commit_message>
<xml_diff>
--- a/Ejercicios/Ejercicios/Planificación.xlsx
+++ b/Ejercicios/Ejercicios/Planificación.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfredo.garcia\Desktop\DocTecnara\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Tecnara\Ejercicios\Ejercicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Ejercicios Enum y DateTime</t>
   </si>
@@ -38,15 +38,9 @@
     <t>Ejercicios BBDD</t>
   </si>
   <si>
-    <t>Explicar Excepciones,  Expresiones Lambda y juego de la ruleta de la suerte</t>
-  </si>
-  <si>
     <t>Dejar tiempo para los ejercicios, corregir y empezar con el juego de la ruleta de la suerte</t>
   </si>
   <si>
-    <t>Explicar expresiones Regex y Linq, y hacer ejercicios</t>
-  </si>
-  <si>
     <t>Temario BBDD y ejercicios</t>
   </si>
   <si>
@@ -65,14 +59,35 @@
     <t>Ejercicios de Hilos y Ruleta de la suerte</t>
   </si>
   <si>
-    <t>Corregir ejercicios</t>
+    <t>Explicar ficheros y Convencion de nombres</t>
+  </si>
+  <si>
+    <t>Explicar Excepciones,  Expresiones Lambda, LINQ y REGEX</t>
+  </si>
+  <si>
+    <t>Explicar principios SOLID y Enums</t>
+  </si>
+  <si>
+    <t>MARZO</t>
+  </si>
+  <si>
+    <t>ABRIL</t>
+  </si>
+  <si>
+    <t>MAYO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Explicar Datetime y ejercicios enum</t>
+  </si>
+  <si>
+    <t>Ejercicios ficheros.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +95,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +135,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -264,10 +304,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -301,16 +342,67 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -320,70 +412,52 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -710,455 +784,491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:P35"/>
+  <dimension ref="A3:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:K21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="13"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+    <row r="3" spans="1:16" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B3" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+    </row>
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+    </row>
+    <row r="6" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="39">
+        <v>44998</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="10">
         <v>45026</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="30"/>
-    </row>
-    <row r="7" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="40">
+        <v>44999</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="11">
         <v>45027</v>
       </c>
-      <c r="H7" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
+      <c r="H7" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
       <c r="L7" s="11">
         <v>45048</v>
       </c>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="22"/>
-    </row>
-    <row r="8" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="16">
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="31"/>
+    </row>
+    <row r="8" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14">
         <v>45000</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="11">
         <v>45028</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
+      <c r="H8" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
       <c r="L8" s="11">
         <v>45049</v>
       </c>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="22"/>
-    </row>
-    <row r="9" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="16">
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="31"/>
+    </row>
+    <row r="9" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14">
         <v>45001</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
+      <c r="C9" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="11">
         <v>45029</v>
       </c>
-      <c r="H9" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
+      <c r="H9" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
       <c r="L9" s="11">
         <v>45050</v>
       </c>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="22"/>
-    </row>
-    <row r="10" spans="1:16" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="11">
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="31"/>
+    </row>
+    <row r="10" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="14">
         <v>45002</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="C10" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="11">
         <v>45030</v>
       </c>
-      <c r="H10" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="22"/>
+      <c r="H10" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="11">
         <v>45051</v>
       </c>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="22"/>
-    </row>
-    <row r="11" spans="1:16" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="31"/>
+    </row>
+    <row r="11" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="33"/>
-    </row>
-    <row r="12" spans="1:16" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="10">
+      <c r="B11" s="18"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="20"/>
+    </row>
+    <row r="12" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="41">
         <v>45005</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
+      <c r="C12" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
       <c r="G12" s="10">
         <v>45033</v>
       </c>
-      <c r="H12" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="10">
+      <c r="H12" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="42">
         <v>45054</v>
       </c>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="22"/>
-    </row>
-    <row r="13" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="11">
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="31"/>
+    </row>
+    <row r="13" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="14">
         <v>45006</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="C13" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="11">
         <v>45034</v>
       </c>
-      <c r="H13" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="11">
+      <c r="H13" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="43">
         <v>45055</v>
       </c>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="22"/>
-    </row>
-    <row r="14" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="11">
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="31"/>
+    </row>
+    <row r="14" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="14">
         <v>45007</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="C14" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="11">
         <v>45035</v>
       </c>
-      <c r="H14" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
+      <c r="H14" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
       <c r="L14" s="11">
         <v>45056</v>
       </c>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="22"/>
-    </row>
-    <row r="15" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="31"/>
+    </row>
+    <row r="15" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11">
         <v>45008</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="11">
         <v>45036</v>
       </c>
-      <c r="H15" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="H15" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
       <c r="L15" s="11">
         <v>45057</v>
       </c>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="22"/>
-    </row>
-    <row r="16" spans="1:16" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="31"/>
+    </row>
+    <row r="16" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>45009</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="11">
         <v>45037</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="H16" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
       <c r="L16" s="11">
         <v>45058</v>
       </c>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="22"/>
-    </row>
-    <row r="17" spans="1:16" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="31"/>
+    </row>
+    <row r="17" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="36"/>
-    </row>
-    <row r="18" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="23"/>
+    </row>
+    <row r="18" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10">
         <v>45012</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
       <c r="L18" s="10">
         <v>45061</v>
       </c>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="22"/>
-    </row>
-    <row r="19" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="31"/>
+    </row>
+    <row r="19" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="11">
         <v>45013</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
       <c r="G19" s="11">
         <v>45041</v>
       </c>
-      <c r="H19" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="H19" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
       <c r="L19" s="11">
         <v>45062</v>
       </c>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="22"/>
-    </row>
-    <row r="20" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="31"/>
+    </row>
+    <row r="20" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
         <v>45014</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
       <c r="G20" s="11">
         <v>45042</v>
       </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="11">
         <v>45063</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="22"/>
-    </row>
-    <row r="21" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="31"/>
+    </row>
+    <row r="21" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
         <v>45015</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="C21" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="11">
         <v>45043</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
       <c r="L21" s="11">
         <v>45064</v>
       </c>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="22"/>
-    </row>
-    <row r="22" spans="1:16" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="31"/>
+    </row>
+    <row r="22" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>45016</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="C22" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
       <c r="G22" s="11">
         <v>45044</v>
       </c>
-      <c r="H22" s="37"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="25"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
       <c r="L22" s="11">
         <v>45065</v>
       </c>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="22"/>
-    </row>
-    <row r="23" spans="1:16" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="31"/>
+    </row>
+    <row r="23" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="36"/>
-    </row>
-    <row r="24" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="23"/>
+    </row>
+    <row r="24" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1173,12 +1283,12 @@
       <c r="L24" s="10">
         <v>45068</v>
       </c>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="22"/>
-    </row>
-    <row r="25" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="31"/>
+    </row>
+    <row r="25" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1193,12 +1303,12 @@
       <c r="L25" s="11">
         <v>45069</v>
       </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="22"/>
-    </row>
-    <row r="26" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="31"/>
+    </row>
+    <row r="26" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1213,12 +1323,12 @@
       <c r="L26" s="11">
         <v>45070</v>
       </c>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="22"/>
-    </row>
-    <row r="27" spans="1:16" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="31"/>
+    </row>
+    <row r="27" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1233,12 +1343,12 @@
       <c r="L27" s="12">
         <v>45071</v>
       </c>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="25"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="26"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F28" s="1"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1249,7 +1359,7 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1260,7 +1370,7 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1270,32 +1380,32 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="6:10" x14ac:dyDescent="0.3">
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F34" s="1"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F35" s="1"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -1303,7 +1413,46 @@
       <c r="J35" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="55">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="M21:P21"/>
     <mergeCell ref="M6:P6"/>
     <mergeCell ref="B11:P11"/>
     <mergeCell ref="B17:P17"/>
@@ -1320,42 +1469,6 @@
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
subida Lunes 27 marzo
</commit_message>
<xml_diff>
--- a/Ejercicios/Ejercicios/Planificación.xlsx
+++ b/Ejercicios/Ejercicios/Planificación.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Ejercicios Enum y DateTime</t>
   </si>
   <si>
-    <t xml:space="preserve">Explicar Ficheros de Texto con CLOSEXML y Linq  </t>
-  </si>
-  <si>
     <t>Hacer Ejercicios de Ficheros y Linq</t>
   </si>
   <si>
@@ -81,6 +78,12 @@
   </si>
   <si>
     <t>Ejercicios ficheros.txt</t>
+  </si>
+  <si>
+    <t>Ejercicios ClosedXML</t>
+  </si>
+  <si>
+    <t>Ejercicios ficheros.txt y explicar ClosedXML</t>
   </si>
 </sst>
 </file>
@@ -346,6 +349,76 @@
     <xf numFmtId="16" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -358,6 +431,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,84 +452,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -786,91 +789,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:K15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="1:16" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
     </row>
     <row r="6" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="39">
+      <c r="B6" s="15">
         <v>44998</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
+      <c r="C6" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
       <c r="G6" s="10">
         <v>45026</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="H6" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
       <c r="L6" s="13"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="17"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="41"/>
     </row>
     <row r="7" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="40">
+      <c r="B7" s="16">
         <v>44999</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
+      <c r="C7" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="11">
         <v>45027</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="H7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
       <c r="L7" s="11">
         <v>45048</v>
       </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
       <c r="P7" s="31"/>
     </row>
     <row r="8" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -886,45 +889,45 @@
       <c r="G8" s="11">
         <v>45028</v>
       </c>
-      <c r="H8" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
+      <c r="H8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
       <c r="L8" s="11">
         <v>45049</v>
       </c>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
       <c r="P8" s="31"/>
     </row>
     <row r="9" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
         <v>45001</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="11">
         <v>45029</v>
       </c>
-      <c r="H9" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
+      <c r="H9" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
       <c r="L9" s="11">
         <v>45050</v>
       </c>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
       <c r="P9" s="31"/>
     </row>
     <row r="10" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -932,7 +935,7 @@
         <v>45002</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
@@ -940,63 +943,63 @@
       <c r="G10" s="11">
         <v>45030</v>
       </c>
-      <c r="H10" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="H10" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
       <c r="K10" s="31"/>
       <c r="L10" s="11">
         <v>45051</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
       <c r="P10" s="31"/>
     </row>
     <row r="11" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="20"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="45"/>
     </row>
     <row r="12" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="41">
+      <c r="B12" s="17">
         <v>45005</v>
       </c>
-      <c r="C12" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="48"/>
+      <c r="C12" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="10">
         <v>45033</v>
       </c>
-      <c r="H12" s="49" t="s">
-        <v>8</v>
+      <c r="H12" s="32" t="s">
+        <v>7</v>
       </c>
       <c r="I12" s="33"/>
       <c r="J12" s="33"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="42">
+      <c r="K12" s="34"/>
+      <c r="L12" s="18">
         <v>45054</v>
       </c>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
       <c r="P12" s="31"/>
     </row>
     <row r="13" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1004,7 +1007,7 @@
         <v>45006</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -1012,18 +1015,18 @@
       <c r="G13" s="11">
         <v>45034</v>
       </c>
-      <c r="H13" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
+      <c r="H13" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
       <c r="K13" s="31"/>
-      <c r="L13" s="43">
+      <c r="L13" s="19">
         <v>45055</v>
       </c>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
       <c r="P13" s="31"/>
     </row>
     <row r="14" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1031,7 +1034,7 @@
         <v>45007</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="27"/>
@@ -1039,234 +1042,234 @@
       <c r="G14" s="11">
         <v>45035</v>
       </c>
-      <c r="H14" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="H14" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="11">
         <v>45056</v>
       </c>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
       <c r="P14" s="31"/>
     </row>
     <row r="15" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="11">
+      <c r="B15" s="14">
         <v>45008</v>
       </c>
-      <c r="C15" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="C15" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="11">
         <v>45036</v>
       </c>
-      <c r="H15" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
+      <c r="H15" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
       <c r="L15" s="11">
         <v>45057</v>
       </c>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
       <c r="P15" s="31"/>
     </row>
     <row r="16" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="11">
+      <c r="B16" s="14">
         <v>45009</v>
       </c>
-      <c r="C16" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="C16" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="11">
         <v>45037</v>
       </c>
-      <c r="H16" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
+      <c r="H16" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
       <c r="L16" s="11">
         <v>45058</v>
       </c>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
       <c r="P16" s="31"/>
     </row>
     <row r="17" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="23"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="48"/>
     </row>
     <row r="18" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10">
+      <c r="B18" s="17">
         <v>45012</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
+      <c r="C18" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
       <c r="L18" s="10">
         <v>45061</v>
       </c>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
       <c r="P18" s="31"/>
     </row>
     <row r="19" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="11">
         <v>45013</v>
       </c>
-      <c r="C19" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
+      <c r="C19" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="11">
         <v>45041</v>
       </c>
-      <c r="H19" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
+      <c r="H19" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
       <c r="L19" s="11">
         <v>45062</v>
       </c>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
       <c r="P19" s="31"/>
     </row>
     <row r="20" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
         <v>45014</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
+      <c r="C20" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="11">
         <v>45042</v>
       </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
       <c r="L20" s="11">
         <v>45063</v>
       </c>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
       <c r="P20" s="31"/>
     </row>
     <row r="21" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
         <v>45015</v>
       </c>
-      <c r="C21" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
+      <c r="C21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="11">
         <v>45043</v>
       </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
       <c r="L21" s="11">
         <v>45064</v>
       </c>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
       <c r="P21" s="31"/>
     </row>
     <row r="22" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>45016</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
+      <c r="C22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="11">
         <v>45044</v>
       </c>
-      <c r="H22" s="24"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="26"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="37"/>
       <c r="L22" s="11">
         <v>45065</v>
       </c>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
       <c r="P22" s="31"/>
     </row>
     <row r="23" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="23"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="48"/>
     </row>
     <row r="24" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
@@ -1283,9 +1286,9 @@
       <c r="L24" s="10">
         <v>45068</v>
       </c>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
       <c r="P24" s="31"/>
     </row>
     <row r="25" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1303,9 +1306,9 @@
       <c r="L25" s="11">
         <v>45069</v>
       </c>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
       <c r="P25" s="31"/>
     </row>
     <row r="26" spans="1:16" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1323,9 +1326,9 @@
       <c r="L26" s="11">
         <v>45070</v>
       </c>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
       <c r="P26" s="31"/>
     </row>
     <row r="27" spans="1:16" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1343,10 +1346,10 @@
       <c r="L27" s="12">
         <v>45071</v>
       </c>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="26"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="37"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F28" s="1"/>
@@ -1414,45 +1417,6 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="M21:P21"/>
     <mergeCell ref="M6:P6"/>
     <mergeCell ref="B11:P11"/>
     <mergeCell ref="B17:P17"/>
@@ -1469,6 +1433,45 @@
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="M14:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>